<commit_message>
add a lot of changes, bot ver 2.0
</commit_message>
<xml_diff>
--- a/files/Direction.xlsx
+++ b/files/Direction.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mihail\PycharmProjects\CDT_bot\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58BEF6A6-1329-4379-98A2-D57662D5EED8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B522D54E-BA56-44BC-8799-A994761AD77E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2138,7 +2138,7 @@
   <dimension ref="A1:K242"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="A244" sqref="A244"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2190,7 +2190,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="33" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="28" t="s">
         <v>0</v>
       </c>
@@ -2295,7 +2295,7 @@
         <v>1373316</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="57" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="57" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="28" t="s">
         <v>0</v>
       </c>
@@ -2330,7 +2330,7 @@
         <v>1598614</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" ht="42.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="28" t="s">
         <v>0</v>
       </c>
@@ -2365,7 +2365,7 @@
         <v>1602795</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" ht="31.15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="28" t="s">
         <v>0</v>
       </c>
@@ -2400,7 +2400,7 @@
         <v>1607665</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="64.150000000000006" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="64.150000000000006" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="28" t="s">
         <v>0</v>
       </c>
@@ -3392,7 +3392,7 @@
       </c>
       <c r="K37" s="21"/>
     </row>
-    <row r="38" spans="1:11" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" s="28" t="s">
         <v>0</v>
       </c>
@@ -3458,7 +3458,7 @@
       </c>
       <c r="K39" s="21"/>
     </row>
-    <row r="40" spans="1:11" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" s="28" t="s">
         <v>0</v>
       </c>
@@ -3788,7 +3788,7 @@
       </c>
       <c r="K49" s="21"/>
     </row>
-    <row r="50" spans="1:11" ht="28.5" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:11" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" s="28" t="s">
         <v>0</v>
       </c>
@@ -3823,7 +3823,7 @@
         <v>582900</v>
       </c>
     </row>
-    <row r="51" spans="1:11" ht="42.75" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:11" ht="42.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" s="28" t="s">
         <v>0</v>
       </c>
@@ -3891,7 +3891,7 @@
       </c>
       <c r="K52" s="21"/>
     </row>
-    <row r="53" spans="1:11" ht="28.5" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:11" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" s="28" t="s">
         <v>115</v>
       </c>
@@ -3926,7 +3926,7 @@
         <v>1601749</v>
       </c>
     </row>
-    <row r="54" spans="1:11" ht="28.5" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:11" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" s="28" t="s">
         <v>115</v>
       </c>
@@ -3961,7 +3961,7 @@
         <v>1601752</v>
       </c>
     </row>
-    <row r="55" spans="1:11" ht="28.5" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:11" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" s="28" t="s">
         <v>115</v>
       </c>
@@ -4031,7 +4031,7 @@
         <v>343839</v>
       </c>
     </row>
-    <row r="57" spans="1:11" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:11" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="28" t="s">
         <v>115</v>
       </c>
@@ -4066,7 +4066,7 @@
         <v>1369524</v>
       </c>
     </row>
-    <row r="58" spans="1:11" ht="28.5" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:11" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" s="28" t="s">
         <v>115</v>
       </c>
@@ -4101,7 +4101,7 @@
         <v>1631158</v>
       </c>
     </row>
-    <row r="59" spans="1:11" ht="28.5" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:11" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" s="28" t="s">
         <v>115</v>
       </c>
@@ -5555,7 +5555,7 @@
       </c>
       <c r="K102" s="21"/>
     </row>
-    <row r="103" spans="1:11" ht="28.5" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:11" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103" s="28" t="s">
         <v>174</v>
       </c>
@@ -5590,7 +5590,7 @@
         <v>1573021</v>
       </c>
     </row>
-    <row r="104" spans="1:11" ht="28.5" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:11" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104" s="28" t="s">
         <v>174</v>
       </c>
@@ -5625,7 +5625,7 @@
         <v>1647013</v>
       </c>
     </row>
-    <row r="105" spans="1:11" ht="28.5" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:11" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105" s="28" t="s">
         <v>174</v>
       </c>
@@ -5660,7 +5660,7 @@
         <v>1368053</v>
       </c>
     </row>
-    <row r="106" spans="1:11" ht="28.5" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:11" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106" s="28" t="s">
         <v>174</v>
       </c>
@@ -5695,7 +5695,7 @@
         <v>1353901</v>
       </c>
     </row>
-    <row r="107" spans="1:11" ht="28.5" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:11" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107" s="28" t="s">
         <v>174</v>
       </c>
@@ -7223,7 +7223,7 @@
         <v>867052</v>
       </c>
     </row>
-    <row r="153" spans="1:11" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:11" ht="28.5" x14ac:dyDescent="0.35">
       <c r="A153" s="28" t="s">
         <v>235</v>
       </c>
@@ -7258,7 +7258,7 @@
         <v>1598445</v>
       </c>
     </row>
-    <row r="154" spans="1:11" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:11" ht="28.5" x14ac:dyDescent="0.35">
       <c r="A154" s="28" t="s">
         <v>235</v>
       </c>
@@ -7293,7 +7293,7 @@
         <v>1654578</v>
       </c>
     </row>
-    <row r="155" spans="1:11" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:11" ht="42.75" x14ac:dyDescent="0.35">
       <c r="A155" s="28" t="s">
         <v>235</v>
       </c>
@@ -7328,7 +7328,7 @@
         <v>1654602</v>
       </c>
     </row>
-    <row r="156" spans="1:11" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:11" ht="28.5" x14ac:dyDescent="0.35">
       <c r="A156" s="28" t="s">
         <v>235</v>
       </c>
@@ -7363,7 +7363,7 @@
         <v>1654077</v>
       </c>
     </row>
-    <row r="157" spans="1:11" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:11" ht="42.75" x14ac:dyDescent="0.35">
       <c r="A157" s="28" t="s">
         <v>235</v>
       </c>
@@ -7398,7 +7398,7 @@
         <v>1646740</v>
       </c>
     </row>
-    <row r="158" spans="1:11" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:11" ht="28.5" x14ac:dyDescent="0.35">
       <c r="A158" s="28" t="s">
         <v>235</v>
       </c>
@@ -7468,7 +7468,7 @@
         <v>163258</v>
       </c>
     </row>
-    <row r="160" spans="1:11" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:11" ht="42.75" x14ac:dyDescent="0.35">
       <c r="A160" s="28" t="s">
         <v>235</v>
       </c>
@@ -7503,7 +7503,7 @@
         <v>1646527</v>
       </c>
     </row>
-    <row r="161" spans="1:11" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:11" ht="28.5" x14ac:dyDescent="0.35">
       <c r="A161" s="28" t="s">
         <v>235</v>
       </c>
@@ -7538,7 +7538,7 @@
         <v>1601153</v>
       </c>
     </row>
-    <row r="162" spans="1:11" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:11" ht="28.5" x14ac:dyDescent="0.35">
       <c r="A162" s="28" t="s">
         <v>235</v>
       </c>
@@ -7573,7 +7573,7 @@
         <v>249343</v>
       </c>
     </row>
-    <row r="163" spans="1:11" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:11" ht="29.45" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A163" s="28" t="s">
         <v>235</v>
       </c>
@@ -7608,7 +7608,7 @@
         <v>168519</v>
       </c>
     </row>
-    <row r="164" spans="1:11" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:11" ht="28.5" x14ac:dyDescent="0.35">
       <c r="A164" s="28" t="s">
         <v>235</v>
       </c>
@@ -7643,7 +7643,7 @@
         <v>1337394</v>
       </c>
     </row>
-    <row r="165" spans="1:11" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:11" ht="28.5" x14ac:dyDescent="0.35">
       <c r="A165" s="28" t="s">
         <v>235</v>
       </c>
@@ -7678,7 +7678,7 @@
         <v>196975</v>
       </c>
     </row>
-    <row r="166" spans="1:11" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:11" ht="42.75" x14ac:dyDescent="0.35">
       <c r="A166" s="28" t="s">
         <v>235</v>
       </c>
@@ -7713,7 +7713,7 @@
         <v>46918</v>
       </c>
     </row>
-    <row r="167" spans="1:11" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:11" ht="42.75" x14ac:dyDescent="0.35">
       <c r="A167" s="28" t="s">
         <v>235</v>
       </c>
@@ -8236,7 +8236,7 @@
         <v>563522</v>
       </c>
     </row>
-    <row r="182" spans="1:11" ht="54.6" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:11" ht="54.6" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A182" s="28" t="s">
         <v>235</v>
       </c>
@@ -8634,7 +8634,7 @@
       </c>
       <c r="K193" s="23"/>
     </row>
-    <row r="194" spans="1:11" ht="54.6" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:11" ht="54.6" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A194" s="28" t="s">
         <v>235</v>
       </c>
@@ -8669,7 +8669,7 @@
         <v>47655</v>
       </c>
     </row>
-    <row r="195" spans="1:11" ht="54.6" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:11" ht="54.6" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A195" s="28" t="s">
         <v>235</v>
       </c>
@@ -8770,7 +8770,7 @@
       </c>
       <c r="K197" s="23"/>
     </row>
-    <row r="198" spans="1:11" ht="54.6" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:11" ht="54.6" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A198" s="28" t="s">
         <v>235</v>
       </c>
@@ -8805,7 +8805,7 @@
         <v>1365338</v>
       </c>
     </row>
-    <row r="199" spans="1:11" ht="54.6" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:11" ht="54.6" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A199" s="28" t="s">
         <v>235</v>
       </c>
@@ -8906,7 +8906,7 @@
       </c>
       <c r="K201" s="23"/>
     </row>
-    <row r="202" spans="1:11" ht="54.6" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:11" ht="54.6" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A202" s="28" t="s">
         <v>235</v>
       </c>
@@ -8941,7 +8941,7 @@
         <v>727191</v>
       </c>
     </row>
-    <row r="203" spans="1:11" ht="54.6" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:11" ht="54.6" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A203" s="28" t="s">
         <v>235</v>
       </c>
@@ -8976,7 +8976,7 @@
         <v>727191</v>
       </c>
     </row>
-    <row r="204" spans="1:11" ht="54.6" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:11" ht="54.6" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A204" s="28" t="s">
         <v>235</v>
       </c>
@@ -9011,7 +9011,7 @@
         <v>1597689</v>
       </c>
     </row>
-    <row r="205" spans="1:11" ht="28.5" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:11" ht="28.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A205" s="28" t="s">
         <v>235</v>
       </c>
@@ -9079,7 +9079,7 @@
       </c>
       <c r="K206" s="23"/>
     </row>
-    <row r="207" spans="1:11" ht="28.5" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:11" ht="28.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A207" s="28" t="s">
         <v>235</v>
       </c>
@@ -9114,7 +9114,7 @@
         <v>1070650</v>
       </c>
     </row>
-    <row r="208" spans="1:11" ht="57" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:11" ht="57" hidden="1" x14ac:dyDescent="0.35">
       <c r="A208" s="28" t="s">
         <v>235</v>
       </c>
@@ -9215,7 +9215,7 @@
       </c>
       <c r="K210" s="23"/>
     </row>
-    <row r="211" spans="1:11" ht="28.5" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:11" ht="28.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A211" s="28" t="s">
         <v>235</v>
       </c>
@@ -9283,7 +9283,7 @@
       </c>
       <c r="K212" s="23"/>
     </row>
-    <row r="213" spans="1:11" ht="28.5" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:11" ht="28.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A213" s="28" t="s">
         <v>235</v>
       </c>
@@ -9351,7 +9351,7 @@
       </c>
       <c r="K214" s="23"/>
     </row>
-    <row r="215" spans="1:11" ht="28.5" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:11" ht="28.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A215" s="28" t="s">
         <v>235</v>
       </c>
@@ -9386,7 +9386,7 @@
         <v>563498</v>
       </c>
     </row>
-    <row r="216" spans="1:11" ht="42.75" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:11" ht="42.75" hidden="1" x14ac:dyDescent="0.35">
       <c r="A216" s="28" t="s">
         <v>235</v>
       </c>
@@ -9421,7 +9421,7 @@
         <v>563501</v>
       </c>
     </row>
-    <row r="217" spans="1:11" ht="28.5" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:11" ht="28.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A217" s="28" t="s">
         <v>235</v>
       </c>
@@ -9753,7 +9753,7 @@
       </c>
       <c r="K226" s="23"/>
     </row>
-    <row r="227" spans="1:11" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:11" ht="71.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A227" s="28" t="s">
         <v>235</v>
       </c>
@@ -9852,7 +9852,7 @@
       </c>
       <c r="K229" s="23"/>
     </row>
-    <row r="230" spans="1:11" ht="57" x14ac:dyDescent="0.35">
+    <row r="230" spans="1:11" ht="57" hidden="1" x14ac:dyDescent="0.35">
       <c r="A230" s="28" t="s">
         <v>235</v>
       </c>
@@ -9887,7 +9887,7 @@
         <v>167391</v>
       </c>
     </row>
-    <row r="231" spans="1:11" ht="57" x14ac:dyDescent="0.35">
+    <row r="231" spans="1:11" ht="57" hidden="1" x14ac:dyDescent="0.35">
       <c r="A231" s="28" t="s">
         <v>235</v>
       </c>
@@ -9922,7 +9922,7 @@
         <v>167391</v>
       </c>
     </row>
-    <row r="232" spans="1:11" ht="57" x14ac:dyDescent="0.35">
+    <row r="232" spans="1:11" ht="57" hidden="1" x14ac:dyDescent="0.35">
       <c r="A232" s="28" t="s">
         <v>235</v>
       </c>
@@ -9957,7 +9957,7 @@
         <v>167391</v>
       </c>
     </row>
-    <row r="233" spans="1:11" ht="57" x14ac:dyDescent="0.35">
+    <row r="233" spans="1:11" ht="57" hidden="1" x14ac:dyDescent="0.35">
       <c r="A233" s="28" t="s">
         <v>235</v>
       </c>
@@ -10025,7 +10025,7 @@
       </c>
       <c r="K234" s="23"/>
     </row>
-    <row r="235" spans="1:11" ht="28.5" x14ac:dyDescent="0.35">
+    <row r="235" spans="1:11" ht="28.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A235" s="28" t="s">
         <v>235</v>
       </c>
@@ -10258,7 +10258,7 @@
       </c>
       <c r="K241" s="23"/>
     </row>
-    <row r="242" spans="1:11" ht="28.5" x14ac:dyDescent="0.35">
+    <row r="242" spans="1:11" ht="28.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A242" s="28" t="s">
         <v>235</v>
       </c>
@@ -10295,13 +10295,14 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:K242" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <filterColumn colId="9">
+    <filterColumn colId="0">
       <filters>
-        <filter val="10"/>
-        <filter val="15"/>
-        <filter val="20"/>
-        <filter val="5"/>
-        <filter val="7"/>
+        <filter val="Художественная направленность"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="7">
+      <filters>
+        <filter val="Нет"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>